<commit_message>
change ExcelDataService to retrieve students name, national ID and status
</commit_message>
<xml_diff>
--- a/studentsList.xlsx
+++ b/studentsList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BaSant\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BaSant\Downloads\studentstatus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68659852-15D9-48E6-B860-E5BF500ACA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37955C80-1042-4CAB-9B1C-3E32460E44AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{8E9C94E5-4230-4E39-A9EF-DBD42556CBE2}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>الاسم</t>
   </si>
@@ -28,117 +28,36 @@
     <t>الرقم القومى</t>
   </si>
   <si>
-    <t>الكلية</t>
-  </si>
-  <si>
-    <t>العنوان</t>
-  </si>
-  <si>
-    <t>التقدير</t>
-  </si>
-  <si>
-    <t>نسبة التقدير</t>
-  </si>
-  <si>
-    <t>تاريخ التقدم</t>
-  </si>
-  <si>
     <t>ملاحظات</t>
   </si>
   <si>
     <t>اميره ماهر محمد ابوليفه</t>
   </si>
   <si>
-    <t>كلية طب الأسنان - بكالوريوس طب الفم والأسنان - المستوى الأول</t>
-  </si>
-  <si>
-    <t>الجيزه - قسم الواحات البحرية - الباويطى</t>
-  </si>
-  <si>
-    <t>جيد جدا</t>
-  </si>
-  <si>
     <t>خديجه خالد صابر عطوه علي</t>
   </si>
   <si>
-    <t>كلية الهندسة - هندسة العمارة والتصميم البيئي - المستوى الثالث</t>
-  </si>
-  <si>
-    <t>الشرقيه - العاشر من رمضان</t>
-  </si>
-  <si>
     <t>دنيا محمد أحمد إبراهيم</t>
   </si>
   <si>
-    <t>كلية طب الأسنان - بكالوريوس طب الفم والأسنان - المستوى الثانى</t>
-  </si>
-  <si>
-    <t>الاسكندريه - البيطاش</t>
-  </si>
-  <si>
-    <t>جيد</t>
-  </si>
-  <si>
     <t>روان أحمد إسماعيل محمد</t>
   </si>
   <si>
-    <t>كلية تكنولوجيا العلوم الصحية التطبيقية - برنامج المختبرات الطبية - المستوى الثانى</t>
-  </si>
-  <si>
-    <t>الدقهلية - السنبلاوين - كفر غنام</t>
-  </si>
-  <si>
     <t>ساره محمد عبدالحميد عبدالهادي</t>
   </si>
   <si>
-    <t>كلية علوم الحاسب وتكنولوجيا المعلومات - علوم البيانات - المستوى الثانى</t>
-  </si>
-  <si>
-    <t>الفيوم - مركز يوسف الصديق - المشرك قبلى</t>
-  </si>
-  <si>
-    <t>مقبول</t>
-  </si>
-  <si>
-    <t>15/8/2024 02:18 PM</t>
-  </si>
-  <si>
     <t>صفاء اشرف محمود عبدالسيد</t>
   </si>
   <si>
-    <t>اسوان - مركز دراو - الجعافرة</t>
-  </si>
-  <si>
-    <t>ناجح</t>
-  </si>
-  <si>
-    <t>18/8/2024 05:13 PM</t>
-  </si>
-  <si>
     <t>منار السيد صبحى حسينى</t>
   </si>
   <si>
-    <t>الشرقيه - مشتول السوق - كفر دهمشا</t>
-  </si>
-  <si>
-    <t>15/8/2024 09:10 AM</t>
-  </si>
-  <si>
     <t>نورهان محمد بكر الصديق علي معوض</t>
   </si>
   <si>
-    <t>كلية العلوم - التكنولوجيا الحيوية والهندسة الوراثية - المستوى الثانى</t>
-  </si>
-  <si>
-    <t>الدقهلية - المطرية - العصافرة</t>
-  </si>
-  <si>
     <t>ولاء عمر حسن عبدالسلام</t>
   </si>
   <si>
-    <t>بنى سويف - ناصر</t>
-  </si>
-  <si>
     <t>لم يستدل عليه</t>
   </si>
   <si>
@@ -167,6 +86,12 @@
   </si>
   <si>
     <t>30503122202344</t>
+  </si>
+  <si>
+    <t>مرفوض</t>
+  </si>
+  <si>
+    <t xml:space="preserve">مقبول لم يستدل </t>
   </si>
 </sst>
 </file>
@@ -1050,25 +975,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFABA9ED-DE39-4B3E-A8F2-B4A3207707C2}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1078,253 +1002,145 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="B2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="B3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="B4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="B5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="B6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="7" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="B8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="B9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2">
-        <v>85.68</v>
-      </c>
-      <c r="G2" s="3">
-        <v>45573.897222222222</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="3">
-        <v>45573.274305555555</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="2">
-        <v>79</v>
-      </c>
-      <c r="G4" s="3">
-        <v>45573.602777777778</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="2">
-        <v>2.78</v>
-      </c>
-      <c r="G5" s="3">
-        <v>45634.924305555556</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="2">
-        <v>63</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="2">
-        <v>70</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="2">
-        <v>82</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="2">
-        <v>75</v>
-      </c>
-      <c r="G9" s="3">
-        <v>45634.838194444441</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="2">
-        <v>74</v>
-      </c>
-      <c r="G10" s="3">
-        <v>45573.449305555558</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>39</v>
-      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Edit the response tp be a json
</commit_message>
<xml_diff>
--- a/studentsList.xlsx
+++ b/studentsList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BaSant\Downloads\studentstatus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37955C80-1042-4CAB-9B1C-3E32460E44AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66C94A6-2482-497B-BCB9-F62536C219A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{8E9C94E5-4230-4E39-A9EF-DBD42556CBE2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{8E9C94E5-4230-4E39-A9EF-DBD42556CBE2}"/>
   </bookViews>
   <sheets>
     <sheet name="studentsList" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
     <t>مرفوض</t>
   </si>
   <si>
-    <t xml:space="preserve">مقبول لم يستدل </t>
+    <t xml:space="preserve">مقبول </t>
   </si>
 </sst>
 </file>
@@ -978,7 +978,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,7 +1007,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>

</xml_diff>